<commit_message>
Plantilla y rows updated
Actualizada la plantilla y las filas ya que hemos añadido la columna Workgroup WA
</commit_message>
<xml_diff>
--- a/PlantillaSTEP4.xlsx
+++ b/PlantillaSTEP4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carnivalcorpeur-my.sharepoint.com/personal/jeremy_lopez_es_costa_it/Documents/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carnivalcorpeur-my.sharepoint.com/personal/jeremy_lopez_es_costa_it/Documents/Documents/GitHub/otropyt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{62065467-E4FB-4B95-9C2F-FD0E7E183FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D67874B3-094A-4851-9BF7-A64AE1D1EB44}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{62065467-E4FB-4B95-9C2F-FD0E7E183FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DC00738-6793-4B71-8FE4-6D576A848600}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -84,6 +106,9 @@
   </si>
   <si>
     <t>D365 email | Default Queue</t>
+  </si>
+  <si>
+    <t>Workgroup WA</t>
   </si>
 </sst>
 </file>
@@ -174,7 +199,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -271,7 +296,46 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -281,28 +345,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -314,7 +370,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -331,9 +387,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
@@ -393,9 +446,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
@@ -408,17 +458,56 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -439,75 +528,68 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>815926</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Immagine 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A104F2B-63B5-4674-967B-C6A797EE042F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="304801" y="201930"/>
-          <a:ext cx="749885" cy="557145"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="0070C0"/>
-          </a:solidFill>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -773,13 +855,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649147B9-A037-4F5A-995A-969407D84600}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="W36" sqref="W36"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -787,62 +869,68 @@
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="1.6640625" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.21875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="14" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" style="15" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" customWidth="1"/>
-    <col min="19" max="21" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="39.88671875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" style="38" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
+    <col min="14" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.109375" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
+    <col min="20" max="22" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="5"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:22" s="2" customFormat="1" ht="7.2" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:23" s="2" customFormat="1" ht="7.2" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
+      <c r="C2" s="31" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="27"/>
     </row>
-    <row r="3" spans="1:22" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:23" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="26"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="30" t="s">
         <v>11</v>
       </c>
@@ -857,18 +945,19 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
       <c r="P3" s="30"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="28"/>
     </row>
-    <row r="4" spans="1:22" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:23" ht="19.8" x14ac:dyDescent="0.7">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="26"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="24"/>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
@@ -881,109 +970,114 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="28"/>
     </row>
-    <row r="5" spans="1:22" s="1" customFormat="1" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:23" s="1" customFormat="1" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="29"/>
     </row>
-    <row r="6" spans="1:22" s="17" customFormat="1" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="27" t="s">
+    <row r="6" spans="1:23" s="16" customFormat="1" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>6</v>
+      <c r="H6" s="25" t="s">
+        <v>16</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="19" t="s">
         <v>12</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>13</v>
       </c>
       <c r="N6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="20" t="s">
+      <c r="P6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="28" t="s">
+      <c r="R6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="28" t="s">
+      <c r="S6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="S6" s="20" t="s">
+      <c r="T6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="20" t="s">
+      <c r="U6" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="22" t="s">
+      <c r="V6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="V6" s="23" t="s">
+      <c r="W6" s="22" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E3:P4"/>
+  <mergeCells count="2">
+    <mergeCell ref="E3:Q4"/>
+    <mergeCell ref="C2:C5"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>